<commit_message>
Eliminated one BoM line-item by caving and making the MDIO 10k resistor be size 0402 instead of 0603, to match the million other 10k 0402s.
</commit_message>
<xml_diff>
--- a/jvc43_bom.xlsx
+++ b/jvc43_bom.xlsx
@@ -161,11 +161,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV65536"/>
+  <dimension ref="A1:IV1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -178,7 +178,7 @@
     <col min="6" max="6" style="0" width="25.141346153846158" bestFit="1" customWidth="1"/>
     <col min="7" max="7" style="0" width="8.856610576923078" bestFit="1" customWidth="1"/>
     <col min="8" max="8" style="0" width="10.999338942307693" bestFit="1" customWidth="1"/>
-    <col min="9" max="256" style="0" width="9.142307692307693"/>
+    <col min="9" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256" ht="13.5">
@@ -1079,27 +1079,27 @@
         </is>
       </c>
     </row>
-    <row r="24" spans="1:256">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>R201 R301</t>
+    <row r="24" spans="1:256" ht="64.5">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>R201 R208 R209 R210 R211 R212 R213 R214 R215 R216 R218 R219 R220 R221 R222 R223 R224 R301 R308 R309 R310 R311 R312 R313 R314 R315 R316 R318 R319 R320 R321 R322 R323 R324</t>
         </is>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>ERJ-3EKF1002V</t>
+          <t>ERJ-2RKF1002X</t>
         </is>
       </c>
     </row>
@@ -1151,17 +1151,17 @@
         </is>
       </c>
     </row>
-    <row r="27" spans="1:256" ht="51.75">
-      <c r="A27" s="4" t="inlineStr">
-        <is>
-          <t>R208 R209 R210 R211 R212 R213 R214 R215 R216 R218 R219 R220 R221 R222 R223 R224 R308 R309 R310 R311 R312 R313 R314 R315 R316 R318 R319 R320 R321 R322 R323 R324</t>
+    <row r="27" spans="1:256">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>R217 R317</t>
         </is>
       </c>
       <c r="B27">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1169,47 +1169,47 @@
       <c r="E27" t="s">
         <v>1</v>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>ERJ-2RKF1002X</t>
-        </is>
+      <c r="F27" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:256">
       <c r="A28" t="inlineStr">
         <is>
-          <t>R217 R317</t>
+          <t>R225 R325</t>
         </is>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28" t="s">
-        <v>18</v>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>6.04k</t>
+        </is>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
       </c>
-      <c r="F28" t="s">
-        <v>18</v>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>ERJ-3EKF6041V</t>
+        </is>
       </c>
     </row>
     <row r="29" spans="1:256">
       <c r="A29" t="inlineStr">
         <is>
-          <t>R225 R325</t>
+          <t>R401</t>
         </is>
       </c>
       <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>6.04k</t>
-        </is>
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>2.1000000000000001</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
@@ -1219,21 +1219,23 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ERJ-3EKF6041V</t>
+          <t>ERJ-3GEYJ2R2V</t>
         </is>
       </c>
     </row>
     <row r="30" spans="1:256">
       <c r="A30" t="inlineStr">
         <is>
-          <t>R401</t>
+          <t>R402 R403</t>
         </is>
       </c>
       <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>2.1000000000000001</v>
+        <v>2</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>5.1k</t>
+        </is>
       </c>
       <c r="D30" t="s">
         <v>17</v>
@@ -1243,22 +1245,22 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ERJ-3GEYJ2R2V</t>
+          <t>ERJ-3EKF5101V</t>
         </is>
       </c>
     </row>
     <row r="31" spans="1:256">
       <c r="A31" t="inlineStr">
         <is>
-          <t>R402 R403</t>
+          <t>R404</t>
         </is>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>5.1k</t>
+          <t>84.5k</t>
         </is>
       </c>
       <c r="D31" t="s">
@@ -1269,14 +1271,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ERJ-3EKF5101V</t>
-        </is>
+          <t>ERJ-3EKF8452V</t>
+        </is>
+      </c>
+      <c r="H31">
+        <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="1:256">
       <c r="A32" t="inlineStr">
         <is>
-          <t>R404</t>
+          <t>R405</t>
         </is>
       </c>
       <c r="B32">
@@ -1284,7 +1289,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>84.5k</t>
+          <t>316k</t>
         </is>
       </c>
       <c r="D32" t="s">
@@ -1295,7 +1300,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ERJ-3EKF8452V</t>
+          <t>ERJ-3EKF3163V</t>
         </is>
       </c>
       <c r="H32">
@@ -1305,15 +1310,15 @@
     <row r="33" spans="1:256">
       <c r="A33" t="inlineStr">
         <is>
-          <t>R405</t>
+          <t>R406 R407</t>
         </is>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>316k</t>
+          <t>100k</t>
         </is>
       </c>
       <c r="D33" t="s">
@@ -1324,7 +1329,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>ERJ-3EKF3163V</t>
+          <t>ERJ-3EKF1003V</t>
         </is>
       </c>
       <c r="H33">
@@ -1334,82 +1339,78 @@
     <row r="34" spans="1:256">
       <c r="A34" t="inlineStr">
         <is>
-          <t>R406 R407</t>
+          <t>TR201 TR301</t>
         </is>
       </c>
       <c r="B34">
         <v>2</v>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>100k</t>
-        </is>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>ERJ-3EKF1003V</t>
-        </is>
-      </c>
-      <c r="H34">
-        <v>0.01</v>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>myfp:magnetics_PT61020E</t>
+        </is>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:256">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TR201 TR301</t>
+          <t>U201 U301</t>
         </is>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
-      <c r="C35" t="s">
-        <v>19</v>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>LAN8831</t>
+        </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>myfp:magnetics_PT61020E</t>
-        </is>
-      </c>
-      <c r="F35" t="s">
-        <v>19</v>
+          <t>myfp:QFN-64-1EP_8x8mm_P0.4mm_EP6x6mm_ThermalVias</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>LAN8831-V/Q2A</t>
+        </is>
       </c>
     </row>
     <row r="36" spans="1:256">
       <c r="A36" t="inlineStr">
         <is>
-          <t>U201 U301</t>
+          <t>U401</t>
         </is>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LAN8831</t>
+          <t>LTC3622*DE</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>myfp:QFN-64-1EP_8x8mm_P0.4mm_EP6x6mm_ThermalVias</t>
+          <t>Package_DFN_QFN:DFN-14-1EP_3x4mm_P0.5mm_EP1.7x3.3mm</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>LAN8831-V/Q2A</t>
+          <t>LTC3622IDE#PBF</t>
         </is>
       </c>
     </row>
     <row r="37" spans="1:256">
       <c r="A37" t="inlineStr">
         <is>
-          <t>U401</t>
+          <t>X101</t>
         </is>
       </c>
       <c r="B37">
@@ -1417,50 +1418,28 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LTC3622*DE</t>
+          <t>25 MHz</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Package_DFN_QFN:DFN-14-1EP_3x4mm_P0.5mm_EP1.7x3.3mm</t>
-        </is>
+          <t>Crystal:Crystal_SMD_2520-4Pin_2.5x2.0mm</t>
+        </is>
+      </c>
+      <c r="E37" t="s">
+        <v>1</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>LTC3622IDE#PBF</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" spans="1:256">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>X101</t>
-        </is>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>25 MHz</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Crystal:Crystal_SMD_2520-4Pin_2.5x2.0mm</t>
-        </is>
-      </c>
-      <c r="E38" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
           <t>ECS-2520MV-250-CN-TR</t>
         </is>
       </c>
     </row>
-    <row r="65536" spans="1:256">
-      <c r="B65536" s="0"/>
+    <row r="65535" spans="1:256">
+      <c r="B65535" s="0"/>
+    </row>
+    <row r="1048576" spans="1:256">
+      <c r="B1048576" s="0"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Re-calculated my power budget for the new PHY chips.  It went waaaay down! - The switcher output caps are slight overkill but are okay to stay as-is - The inductors definitely needed to be increased in value
</commit_message>
<xml_diff>
--- a/jvc43_bom.xlsx
+++ b/jvc43_bom.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21" count="21">
   <si>
     <t>Capacitor_SMD:C_0402_1005Metric</t>
   </si>
@@ -63,13 +63,16 @@
     <t>CGA3E1X7R1E105K080AC</t>
   </si>
   <si>
+    <t>6.2uH</t>
+  </si>
+  <si>
     <t>myfp:L_5.8x5.8mm_cutcir_6.3mm</t>
   </si>
   <si>
+    <t>SRR5028-6R2Y</t>
+  </si>
+  <si>
     <t>Resistor_SMD:R_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>10k</t>
   </si>
   <si>
     <t>Resistor_SMD:R_0603_1608Metric</t>
@@ -164,8 +167,8 @@
   <dimension ref="A1:IV1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1003,7 +1006,7 @@
         </is>
       </c>
     </row>
-    <row r="21" spans="1:256">
+    <row r="21" spans="1:256" ht="13.5">
       <c r="A21" t="inlineStr">
         <is>
           <t>L402</t>
@@ -1012,24 +1015,20 @@
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>4.2uH</t>
-        </is>
+      <c r="C21" t="s">
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
         <v>1</v>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>SRR5028-4R2Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" spans="1:256">
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:256" ht="13.5">
       <c r="A22" t="inlineStr">
         <is>
           <t>L403</t>
@@ -1040,18 +1039,18 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6.2uH</t>
+          <t>15uH</t>
         </is>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
         <v>1</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>SRR5028-6R2Y</t>
+          <t>SRR5028-150Y</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1067,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
@@ -1088,11 +1087,13 @@
       <c r="B24">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
-        <v>16</v>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>10k</t>
+        </is>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s">
         <v>1</v>
@@ -1116,7 +1117,7 @@
         <v>220</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" t="s">
         <v>1</v>
@@ -1140,7 +1141,7 @@
         <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
         <v>1</v>
@@ -1161,16 +1162,16 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:256">
@@ -1188,7 +1189,7 @@
         </is>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E28" t="s">
         <v>1</v>
@@ -1212,7 +1213,7 @@
         <v>2.1000000000000001</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29" t="s">
         <v>1</v>
@@ -1238,7 +1239,7 @@
         </is>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E30" t="s">
         <v>1</v>
@@ -1264,7 +1265,7 @@
         </is>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
         <v>1</v>
@@ -1293,7 +1294,7 @@
         </is>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" t="s">
         <v>1</v>
@@ -1322,7 +1323,7 @@
         </is>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
         <v>1</v>
@@ -1346,7 +1347,7 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1354,7 +1355,7 @@
         </is>
       </c>
       <c r="F34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:256">

</xml_diff>